<commit_message>
Initial commit to main branch
</commit_message>
<xml_diff>
--- a/TestData/MiniProjectExcecutionOutput.xlsx
+++ b/TestData/MiniProjectExcecutionOutput.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="30">
   <si>
     <t>Months</t>
   </si>
@@ -436,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
@@ -1270,6 +1270,158 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="I29" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J29" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="K29" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="L29" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="M29" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N29" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="O29" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="P29" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="J31" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="L31" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="M31" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N31" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="O31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="P31" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>